<commit_message>
Rerun to ensure the operation of Scoring.py
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -496,22 +496,22 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Swim Distance (Yards) StdDev</t>
+          <t>Swim Distance (Yards) std_dev</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Bike Distance (Miles) StdDev</t>
+          <t>Bike Distance (Miles) std_dev</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Run Distance (Miles) StdDev</t>
+          <t>Run Distance (Miles) std_dev</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>averageStdDev</t>
+          <t>average_std_dev</t>
         </is>
       </c>
     </row>

</xml_diff>